<commit_message>
Adam's changes to Analysis1.Rmd
</commit_message>
<xml_diff>
--- a/data/op_2007_16/par.xlsx
+++ b/data/op_2007_16/par.xlsx
@@ -1,21 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlade\Documents\Github\AnalysisPLBIreland\data\op_2007_16\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/U8004755/Development/AnalysisPLBIreland/data/op_2007_16/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42DF7F2-4631-4EA5-8115-01469045AE6F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="18880" windowHeight="6960"/>
   </bookViews>
   <sheets>
     <sheet name="par" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -23,9 +30,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>rh_thresh</t>
-  </si>
-  <si>
-    <t>temp_thres</t>
   </si>
   <si>
     <t>hours</t>
@@ -36,11 +40,14 @@
   <si>
     <t>rain</t>
   </si>
+  <si>
+    <t>temp_thresh</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -875,30 +882,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A49D639C-7226-4915-9077-348B3C3E9338}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>93</v>
       </c>
@@ -909,10 +916,10 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>92</v>
       </c>
@@ -926,7 +933,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>91</v>
       </c>
@@ -937,7 +944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>90</v>
       </c>
@@ -948,7 +955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>89</v>
       </c>
@@ -959,7 +966,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>88</v>
       </c>
@@ -970,7 +977,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>87</v>
       </c>
@@ -981,28 +988,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B26" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in the structure after adams comments
</commit_message>
<xml_diff>
--- a/data/op_2007_16/par.xlsx
+++ b/data/op_2007_16/par.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlade\Documents\Github\AnalysisPLBIreland\data\op_2007_16\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42DF7F2-4631-4EA5-8115-01469045AE6F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3134B8D-28CB-49FF-8E41-C6EC772BDD40}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,6 @@
     <t>rh_thresh</t>
   </si>
   <si>
-    <t>temp_thres</t>
-  </si>
-  <si>
     <t>hours</t>
   </si>
   <si>
@@ -35,6 +32,9 @@
   </si>
   <si>
     <t>rain</t>
+  </si>
+  <si>
+    <t>temp_thresh</t>
   </si>
 </sst>
 </file>
@@ -879,26 +879,26 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>93</v>
       </c>
@@ -909,10 +909,10 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>92</v>
       </c>
@@ -926,7 +926,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>91</v>
       </c>
@@ -937,7 +937,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>90</v>
       </c>
@@ -948,7 +948,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>89</v>
       </c>
@@ -959,7 +959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>88</v>
       </c>
@@ -970,7 +970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>87</v>
       </c>
@@ -981,28 +981,28 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
   </sheetData>

</xml_diff>